<commit_message>
Added code for Test Cases sync to Test Manager
</commit_message>
<xml_diff>
--- a/Input/Requirements.xlsx
+++ b/Input/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashraya.hd\Documents\UiPath\AutomatedTestCaseGeneration\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/arshad_shaikh_uipath_com/Documents/Documents/AutomatedTestGeneration/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DBAB46-3861-428A-A232-8E9EA178F41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40ECC8E4-0B7E-420B-82E4-7F9C641F0778}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="15980" windowHeight="7780" xr2:uid="{40ECC8E4-0B7E-420B-82E4-7F9C641F0778}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -753,23 +753,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26ED0E9A-C600-41F5-A389-BF28116EA69E}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -795,7 +795,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -845,7 +845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -871,7 +871,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -897,7 +897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -921,7 +921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -945,7 +945,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -969,7 +969,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -995,7 +995,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Defaulted in_ExcelUploaded to false
</commit_message>
<xml_diff>
--- a/Input/Requirements.xlsx
+++ b/Input/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashraya.hd\Documents\UiPath\AutomatedTestCaseGeneration\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/arshad_shaikh_uipath_com/Documents/Documents/AutomatedTestGeneration/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B33242-8E09-4BC8-8F26-2FDDC5087804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40ECC8E4-0B7E-420B-82E4-7F9C641F0778}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{40ECC8E4-0B7E-420B-82E4-7F9C641F0778}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -483,22 +483,22 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -524,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>9</v>
       </c>
@@ -550,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>10</v>
       </c>

</xml_diff>